<commit_message>
attempt to fix csv file
</commit_message>
<xml_diff>
--- a/CAD Technology Radar.xlsx
+++ b/CAD Technology Radar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atitarenko/Documents/Code/TechRadar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3110B5-5508-8741-ACAA-E0F6F1B06A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34A86CE-519C-ED4E-845D-ECB8DEAF2498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,17 +397,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -630,16 +633,17 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="51.5" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,210 +656,210 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="5" t="b">
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="5" t="b">
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="5" t="b">
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="5" t="b">
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="5" t="b">
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="5" t="b">
+      <c r="C7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="5" t="b">
+      <c r="C8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="5" t="b">
+      <c r="B10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="5" t="b">
+      <c r="C11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="5" t="b">
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="13">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="5" t="b">
+      <c r="B13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="13">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="6" t="b">
+      <c r="B14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="5" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="13">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D15" t="b">
@@ -863,13 +867,13 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="B16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D16" t="b">
@@ -877,13 +881,13 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="B17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D17" t="b">
@@ -891,13 +895,13 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="B18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D18" t="b">
@@ -905,13 +909,13 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D19" t="b">
@@ -919,13 +923,13 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="B20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D20" t="b">
@@ -933,13 +937,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D21" t="b">
@@ -947,69 +951,69 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="5" t="b">
+      <c r="D22" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="B23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="5" t="b">
+      <c r="D23" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="6" t="b">
+      <c r="D24" s="5" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="5" t="b">
+      <c r="D25" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="B26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D26" t="b">
@@ -1017,13 +1021,13 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="6" t="s">
+      <c r="B27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D27" t="b">
@@ -1031,13 +1035,13 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="6" t="s">
+      <c r="B28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D28" t="b">
@@ -1045,49 +1049,49 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A29" s="4" t="str">
+      <c r="A29" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/techniques/design-systems","Design systems")</f>
         <v>Design systems</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="5" t="s">
+      <c r="B29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" s="5" t="s">
+      <c r="D29" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="5" t="s">
+      <c r="B30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" s="5"/>
+      <c r="D30" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" s="9"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="5" t="s">
+      <c r="B31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="5" t="b">
+      <c r="D31" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E31" s="7" t="s">
@@ -1095,52 +1099,52 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A32" s="4" t="str">
+      <c r="A32" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/techniques/design-system-decision-records","Design system decision records")</f>
         <v>Design system decision records</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="5" t="s">
+      <c r="B32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="5" t="b">
+      <c r="D32" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="9" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A33" s="4" t="str">
+      <c r="A33" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/techniques/llm-powered-autonomous-agents","LLM-powered autonomous agents")</f>
         <v>LLM-powered autonomous agents</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="5" t="b">
+      <c r="D33" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="5" t="b">
+      <c r="D34" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E34" s="7" t="s">
@@ -1148,44 +1152,44 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="6" t="s">
+      <c r="B35" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="6" t="s">
+      <c r="B36" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="6" t="b">
+      <c r="D36" s="5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="6" t="s">
+      <c r="B37" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D37" t="b">
@@ -1196,10 +1200,10 @@
       <c r="A38" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="6" t="s">
+      <c r="B38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D38" t="b">
@@ -1207,30 +1211,30 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D39" t="b">
         <v>1</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="E39" s="10" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="6" t="s">
+      <c r="B40" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D40" t="b">
@@ -1238,30 +1242,30 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="6" t="s">
+      <c r="B41" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E41" s="10" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="6" t="s">
+      <c r="B42" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="b">
@@ -1269,13 +1273,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="6" t="s">
+      <c r="B43" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D43" t="b">
@@ -1283,34 +1287,34 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A44" s="4" t="str">
+      <c r="A44" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/languages-and-frameworks/kotlin-kover","Kotlin Kover")</f>
         <v>Kotlin Kover</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D44" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" s="5" t="s">
+      <c r="B44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D45" s="5" t="b">
+      <c r="B45" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E45" s="7" t="s">
@@ -1318,197 +1322,197 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A46" s="4" t="str">
+      <c r="A46" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/tools/maestro","Maestro")</f>
         <v>Maestro</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" s="5" t="b">
+      <c r="C46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A47" s="4" t="str">
+      <c r="A47" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/tools/openrewrite","OpenRewrite")</f>
         <v>OpenRewrite</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D47" s="5" t="b">
+      <c r="C47" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A48" s="4" t="str">
+      <c r="A48" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/tools/github-copilot","GitHub Copilot")</f>
         <v>GitHub Copilot</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E48" s="5" t="s">
+      <c r="B48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A49" s="4" t="str">
+      <c r="A49" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/tools/chatgpt","ChatGPT")</f>
         <v>ChatGPT</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D49" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E49" s="5" t="s">
+      <c r="B49" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E49" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50" s="5" t="b">
+      <c r="C50" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B51" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D51" s="5" t="b">
+      <c r="B51" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D52" s="5" t="b">
+      <c r="B52" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C53" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D53" s="5" t="b">
+      <c r="C53" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B54" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D54" s="6" t="b">
+      <c r="B54" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="5" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D55" s="6" t="b">
+      <c r="B55" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="5" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D56" s="6" t="b">
+      <c r="C56" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B57" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D57" s="6" t="b">
+      <c r="B57" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58" s="6" t="s">
+      <c r="B58" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D58" t="b">
@@ -1516,13 +1520,13 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="6" t="s">
+      <c r="B59" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D59" t="b">
@@ -1530,13 +1534,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" s="6" t="s">
+      <c r="B60" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D60" t="b">
@@ -1544,13 +1548,13 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B61" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="6" t="s">
+      <c r="B61" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D61" t="b">
@@ -1558,13 +1562,13 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B62" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C62" s="6" t="s">
+      <c r="B62" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D62" t="b">
@@ -1572,13 +1576,13 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D63" t="b">
@@ -1586,13 +1590,13 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B64" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64" s="6" t="s">
+      <c r="B64" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D64" t="b">
@@ -1600,13 +1604,13 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B65" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C65" s="6" t="s">
+      <c r="B65" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D65" t="b">
@@ -1614,13 +1618,13 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B66" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C66" s="6" t="s">
+      <c r="B66" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D66" t="b">
@@ -1628,13 +1632,13 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A67" s="4" t="s">
+      <c r="A67" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B67" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C67" s="6" t="s">
+      <c r="B67" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D67" t="b">
@@ -1642,13 +1646,13 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C68" s="6" t="s">
+      <c r="B68" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D68" t="b">
@@ -1656,13 +1660,13 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A69" s="4" t="s">
+      <c r="A69" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B69" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="6" t="s">
+      <c r="B69" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D69" t="b">
@@ -1670,13 +1674,13 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A70" s="4" t="s">
+      <c r="A70" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B70" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C70" s="6" t="s">
+      <c r="B70" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D70" t="b">
@@ -1684,13 +1688,13 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B71" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="6" t="s">
+      <c r="B71" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D71" t="b">
@@ -1698,13 +1702,13 @@
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A72" s="4" t="s">
+      <c r="A72" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C72" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D72" t="b">

</xml_diff>

<commit_message>
v0.2 updated architectures and removed obvious platforms
</commit_message>
<xml_diff>
--- a/CAD Technology Radar.xlsx
+++ b/CAD Technology Radar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atitarenko/Documents/Code/TechRadar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34A86CE-519C-ED4E-845D-ECB8DEAF2498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74A4D48-9354-DF42-B3D2-4734DC10C95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="89">
   <si>
     <t>name</t>
   </si>
@@ -60,9 +60,6 @@
 &lt;p&gt;Our experiences show that teams seldom apply a product-centric mindset when building design systems. The primary consumers of the shared libraries and documents are the product development teams. When applying a product mindset, system owners should establish empathy with internal consumers (the development teams) and collaborate with them. We've found that the reason many component libraries are maligned is because the owning team wasn't able to give consumers what they needed fast enough and wasn't set up to take outside contributions. A product-centric mindset also requires organizations to think about if and how contributions should be made to the design system and how these contributions should be governed — on this topic, we recommend applying the &lt;a href="/radar/techniques/design-system-decision-records"&gt;design system decision records&lt;/a&gt; technique. For us, running a good design system or component library requires social work as much as technical work.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>tag</t>
-  </si>
-  <si>
     <t>Trial</t>
   </si>
   <si>
@@ -75,16 +72,10 @@
     <t>Hold</t>
   </si>
   <si>
-    <t>&lt;p&gt;Since we first mentioned them in 2014, &lt;a href="/radar/platforms/web-components-standard"&gt;web components&lt;/a&gt; have become popular, and, on the whole, our experience has been positive. Similarly, we've voiced our support for rendering HTML on the server by cautioning against &lt;a href="/radar/techniques/spa-by-default"&gt;SPA by default&lt;/a&gt; and by including frameworks such as &lt;a href="/radar/languages-and-frameworks/next-js"&gt;Next.js&lt;/a&gt; and &lt;a href="/radar/languages-and-frameworks/htmx"&gt;htmx&lt;/a&gt; in addition to traditional server-side frameworks. However, although it’s possible to combine both, it can also prove deeply problematic; that’s why we suggest avoiding &lt;strong&gt;web components for server-side-rendered (SSR) web apps&lt;/strong&gt;. As a browser technology, it's not trivial to use web components on the server. Frameworks have sprung up to make this easier, sometimes even using a browser engine, but the complexity is still there. Worse than the issues with developer experience is the user experience: Page load performance is impacted when custom web components have to be loaded and hydrated in the browser, and even with pre-rendering and careful tweaking of the component, a "flash of unstyled content" or some layout shifting is all but unavoidable. The decision to forgo web components can have far-reaching consequences as one of our teams experienced when they had to move their design system away from the web components–based &lt;a href="/radar/languages-and-frameworks/stencil"&gt;Stencil&lt;/a&gt;.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>Platforms</t>
   </si>
   <si>
     <t>Tools</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;&lt;a href="https://snyk.io/"&gt;Snyk&lt;/a&gt;&lt;/strong&gt; provides both static application security testing (SAST) and software component analysis (SCA) tests to help you find, fix and monitor security issues throughout the software development lifecycle. Its broad range of features is designed to speed up the feedback loop, favoring a shift-left approach instead of the &lt;a href="/radar/techniques/security-sandwich"&gt;security sandwich&lt;/a&gt; anti-pattern. As one of the best security platforms available today, Snyk stands out because of its ability to identify a wider range of issues, enabled mainly by a &lt;a href="https://docs.snyk.io/scan-application-code/snyk-open-source/starting-to-fix-vulnerabilities/using-the-snyk-vulnerability-database"&gt;dedicated research team adding to its vulnerability database&lt;/a&gt;. But there’s room for improvement: the dashboard currently doesn't provide an easy way to filter noise down to specific actionable information; depending on the language ecosystem, SCA-based integrations can output false positives compared to pipeline-based integrations because Snyk has to guess what the resolved dependencies are; automated resolution is not consistently successful; and significant integration investment is required in order to achieve proper gatekeeping or to establish an &lt;a href="/radar/techniques/software-bill-of-materials"&gt;SBOM&lt;/a&gt; in high regulatory environments. Despite these shortcomings, many of our enterprise clients have adopted Snyk; we too are using it for our IT function.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;strong&gt;&lt;a href="https://github.com/features/copilot"&gt;GitHub Copilot&lt;/a&gt;&lt;/strong&gt; is used by many of our teams to help them write code faster. Overall, most of our developers find it very useful and would be cross if we took it away from them. We've been collating and sharing many of our experiences with Copilot through &lt;a href="https://martinfowler.com/articles/exploring-gen-ai.html"&gt;a series on Generative AI&lt;/a&gt; and &lt;a href="https://www.thoughtworks.com/insights/blog/generative-ai/getting-started-with-github-copilot"&gt;a guide on getting started with Copilot&lt;/a&gt;. Note that GitHub Copilot can be used with any codebase, not just codebases hosted on GitHub.&lt;/p&gt;
@@ -104,12 +95,6 @@
     <t>languages-and-frameworks</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;strong&gt;&lt;a href="https://dart.dev/"&gt;Dart&lt;/a&gt;&lt;/strong&gt; is a programming language developed by Google that supports building apps targeting multiple platforms, including web browsers, &lt;a href="/radar/languages-and-frameworks/webassembly"&gt;WebAssembly&lt;/a&gt;, desktop and mobile apps. Its adoption has been driven by the dominance of &lt;a href="/radar/languages-and-frameworks/flutter"&gt;Flutter&lt;/a&gt; — a popular, multi-platform UI toolkit powered by Dart — in the cross-platform native mobile app framework space. In response to community feedback, Dart has evolved since its initial versions and has added built-in &lt;a href="https://dart.dev/null-safety"&gt;sound null safety&lt;/a&gt; in version three, in addition to a robust type system. Furthermore, Dart's ecosystem is growing rapidly, with a vibrant community and a wide range of available libraries and tools, making it attractive for developers.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;&lt;a href="https://github.com/vektra/mockery"&gt;Mockery&lt;/a&gt;&lt;/strong&gt; is a mature &lt;a href="/radar/languages-and-frameworks/go-language"&gt;Golang&lt;/a&gt; library that helps generate mock implementations of interfaces and simulates the behavior of external dependencies. With type-safe methods to generate call expectations and flexible ways to mock return values, it enables the tests to focus on the business logic rather than worrying about the correctness of external dependencies. Mockery uses Go generators and simplifies the generation and management of the mocks in the test suite.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;&lt;a href="https://github.com/Kotlin/kotlinx-kover"&gt;&lt;strong&gt;Kotlin Kover&lt;/strong&gt;&lt;/a&gt; is a code coverage tool set designed specifically for &lt;a href="/radar/languages-and-frameworks/kotlin"&gt;Kotlin&lt;/a&gt;, supporting Kotlin JVM, &lt;a href="/radar/languages-and-frameworks/kotlin-multiplatform-mobile"&gt;Multiplatform&lt;/a&gt; and Android projects. The significance of code coverage lies in its ability to spotlight untested segments, which reinforces software reliability. As Kover evolves, it stands out because of its ability to produce comprehensive HTML and XML reports, coupled with unmatched precision tailored to Kotlin. For teams deeply rooted in Kotlin, we advise you to assess Kover to leverage its potential in enhancing code quality.&lt;/p&gt;</t>
   </si>
   <si>
@@ -143,15 +128,9 @@
     <t>SwiftUI</t>
   </si>
   <si>
-    <t>Compose</t>
-  </si>
-  <si>
     <t>Mockk</t>
   </si>
   <si>
-    <t>Hilt</t>
-  </si>
-  <si>
     <t>MVVM</t>
   </si>
   <si>
@@ -182,21 +161,12 @@
     <t>Renovate</t>
   </si>
   <si>
-    <t>App Modularization</t>
-  </si>
-  <si>
-    <t>Composable Architecture (TCA)</t>
-  </si>
-  <si>
     <t>GenAI powered UI</t>
   </si>
   <si>
     <t>Cross Funktional Team - Backend+Web+App</t>
   </si>
   <si>
-    <t>https://docs.gradle.org/current/userguide/platforms.html</t>
-  </si>
-  <si>
     <t>CodiumAI</t>
   </si>
   <si>
@@ -209,9 +179,6 @@
     <t>Cloud CI/CD</t>
   </si>
   <si>
-    <t>Thread Modelling, OWASP Top 10, Security Champion</t>
-  </si>
-  <si>
     <t>SPM</t>
   </si>
   <si>
@@ -221,18 +188,12 @@
     <t>fastlane</t>
   </si>
   <si>
-    <t>Combine</t>
-  </si>
-  <si>
     <t>ReactiveX</t>
   </si>
   <si>
     <t>LeakCanary</t>
   </si>
   <si>
-    <t>Coroutines</t>
-  </si>
-  <si>
     <t>Espresso</t>
   </si>
   <si>
@@ -281,9 +242,6 @@
     <t>AssertJ</t>
   </si>
   <si>
-    <t>&lt;p&gt;In a fast-paced product development environment where users' needs constantly evolve, design is an area that is ever-changing. This means input on design decisions will continue to be required. Borrowing from the idea of documenting architecture decisions via ADRs, we started adopting a similar format — &lt;strong&gt;design system decision records&lt;/strong&gt; — in order to document design system decisions with the corresponding rationale, research insights and experiment results. Communicating design system decisions effectively seems to be an emerging need of product development teams; doing it in this light manner is also recommended by &lt;a href="https://zeroheight.com/blog/capturing-your-design-system-decisions/"&gt;zeroheight&lt;/a&gt;. This technique helped us reduce onboarding times, move conversations forward and align work streams that share the same design system.&lt;/p&gt;https://cognitect.com/blog/2011/11/15/documenting-architecture-decisions</t>
-  </si>
-  <si>
     <t>Structured Logging</t>
   </si>
   <si>
@@ -308,13 +266,44 @@
     <t>Jackson</t>
   </si>
   <si>
-    <t>Android</t>
-  </si>
-  <si>
-    <t>iOS</t>
-  </si>
-  <si>
-    <t>Huawei</t>
+    <t>Redux</t>
+  </si>
+  <si>
+    <t>MVP</t>
+  </si>
+  <si>
+    <t>VIPER</t>
+  </si>
+  <si>
+    <t>Clean Architecture</t>
+  </si>
+  <si>
+    <t>Modular Architecture</t>
+  </si>
+  <si>
+    <t>A/B Testing</t>
+  </si>
+  <si>
+    <t>Jetpack Compose</t>
+  </si>
+  <si>
+    <t>Jetpack Hilt</t>
+  </si>
+  <si>
+    <t>Kotlin Coroutine</t>
+  </si>
+  <si>
+    <t>Swift Combine</t>
+  </si>
+  <si>
+    <t>TCA</t>
+  </si>
+  <si>
+    <t>Thread Modelling, OWASP Top 10, Security Champion, …</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;In a fast-paced product development environment where users' needs constantly evolve, design is an area that is ever-changing. This means input on design decisions will continue to be required. Borrowing from the idea of documenting architecture decisions via ADRs, we started adopting a similar format — &lt;strong&gt;design system decision records&lt;/strong&gt; — in order to document design system decisions with the corresponding rationale, research insights and experiment results. Communicating design system decisions effectively seems to be an emerging need of product development teams; doing it in this light manner is also recommended by &lt;a href="https://zeroheight.com/blog/capturing-your-design-system-decisions/"&gt;zeroheight&lt;/a&gt;. This technique helped us reduce onboarding times, move conversations forward and align work streams that share the same design system.&lt;/p&gt; 
+https://cognitect.com/blog/2011/11/15/documenting-architecture-decisions</t>
   </si>
 </sst>
 </file>
@@ -397,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -411,6 +400,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -629,18 +621,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="51.5" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="8"/>
+    <col min="5" max="5" width="130.33203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17">
@@ -662,34 +654,30 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D2" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="E2" s="7"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" s="4" t="b">
         <v>0</v>
@@ -697,13 +685,13 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" s="4" t="b">
         <v>0</v>
@@ -711,13 +699,13 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" s="4" t="b">
         <v>0</v>
@@ -725,13 +713,13 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" s="4" t="b">
         <v>0</v>
@@ -739,13 +727,13 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7" s="4" t="b">
         <v>0</v>
@@ -753,13 +741,13 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8" s="4" t="b">
         <v>0</v>
@@ -767,30 +755,28 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" s="4" t="b">
         <v>0</v>
@@ -798,13 +784,13 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" s="4" t="b">
         <v>0</v>
@@ -812,13 +798,13 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D12" s="4" t="b">
         <v>0</v>
@@ -826,13 +812,13 @@
     </row>
     <row r="13" spans="1:7" ht="13">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D13" s="4" t="b">
         <v>0</v>
@@ -840,13 +826,13 @@
     </row>
     <row r="14" spans="1:7" ht="13">
       <c r="A14" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D14" s="5" t="b">
         <v>0</v>
@@ -854,13 +840,13 @@
     </row>
     <row r="15" spans="1:7" ht="13">
       <c r="A15" s="3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -868,13 +854,13 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -882,13 +868,13 @@
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
@@ -896,13 +882,13 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -910,13 +896,13 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
@@ -924,13 +910,13 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -938,13 +924,13 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D21" t="b">
         <v>1</v>
@@ -952,13 +938,13 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D22" s="4" t="b">
         <v>0</v>
@@ -966,13 +952,13 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D23" s="4" t="b">
         <v>1</v>
@@ -980,13 +966,13 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D24" s="5" t="b">
         <v>0</v>
@@ -994,13 +980,13 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="D25" s="4" t="b">
         <v>0</v>
@@ -1008,68 +994,65 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" t="b">
+        <v>12</v>
+      </c>
+      <c r="D26" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" t="b">
+        <v>12</v>
+      </c>
+      <c r="D27" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" t="b">
+        <v>12</v>
+      </c>
+      <c r="D28" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A29" s="3" t="str">
+      <c r="A29" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A30" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/techniques/design-systems","Design systems")</f>
         <v>Design systems</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A30" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="B30" s="4" t="s">
         <v>5</v>
       </c>
@@ -1079,11 +1062,13 @@
       <c r="D30" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E30" s="9"/>
+      <c r="E30" s="9" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>5</v>
@@ -1094,52 +1079,50 @@
       <c r="D31" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>57</v>
-      </c>
+      <c r="E31" s="9"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A32" s="3" t="str">
+      <c r="A32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A33" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/techniques/design-system-decision-records","Design system decision records")</f>
         <v>Design system decision records</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="B33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="4" t="b">
+      <c r="D33" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E32" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A33" s="3" t="str">
+      <c r="E33" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A34" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/techniques/llm-powered-autonomous-agents","LLM-powered autonomous agents")</f>
         <v>LLM-powered autonomous agents</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A34" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="B34" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>6</v>
@@ -1147,61 +1130,59 @@
       <c r="D34" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E34" s="7" t="s">
-        <v>13</v>
+      <c r="E34" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D35" t="b">
+      <c r="D35" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E35" s="8" t="s">
-        <v>52</v>
-      </c>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="5" t="b">
+        <v>12</v>
+      </c>
+      <c r="D36" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D37" t="b">
-        <v>0</v>
+      <c r="D37" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A38" t="s">
-        <v>77</v>
+      <c r="A38" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>6</v>
@@ -1211,25 +1192,22 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A39" s="3" t="s">
-        <v>78</v>
+      <c r="A39" t="s">
+        <v>64</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D39" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>79</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1">
       <c r="A40" s="3" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>9</v>
@@ -1238,15 +1216,18 @@
         <v>6</v>
       </c>
       <c r="D40" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>6</v>
@@ -1254,13 +1235,10 @@
       <c r="D41" t="b">
         <v>0</v>
       </c>
-      <c r="E41" s="10" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1">
       <c r="A42" s="3" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>5</v>
@@ -1271,10 +1249,13 @@
       <c r="D42" t="b">
         <v>0</v>
       </c>
+      <c r="E42" s="10" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1">
       <c r="A43" s="3" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>5</v>
@@ -1287,135 +1268,133 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A44" s="3" t="str">
+      <c r="A44" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A45" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/languages-and-frameworks/kotlin-kover","Kotlin Kover")</f>
         <v>Kotlin Kover</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D44" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A45" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="B45" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="D45" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E45" s="7" t="s">
-        <v>16</v>
+      <c r="E45" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A46" s="3" t="str">
+      <c r="A46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" s="7"/>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A47" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/tools/maestro","Maestro")</f>
         <v>Maestro</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" s="4" t="b">
+      <c r="B47" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E46" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A47" s="3" t="str">
+      <c r="E47" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A48" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/tools/openrewrite","OpenRewrite")</f>
         <v>OpenRewrite</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D47" s="4" t="b">
+      <c r="B48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E47" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A48" s="3" t="str">
+      <c r="E48" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A49" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/tools/github-copilot","GitHub Copilot")</f>
         <v>GitHub Copilot</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A49" s="3" t="str">
+      <c r="B49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A50" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/tools/chatgpt","ChatGPT")</f>
         <v>ChatGPT</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="4" t="s">
+      <c r="B50" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="9" t="s">
         <v>15</v>
-      </c>
-      <c r="D49" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A50" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50" s="4" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="D51" s="4" t="b">
         <v>0</v>
@@ -1423,55 +1402,55 @@
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D52" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A53" s="5" t="s">
-        <v>75</v>
+      <c r="A53" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D53" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A54" s="3" t="s">
-        <v>43</v>
+      <c r="A54" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D54" s="5" t="b">
+        <v>13</v>
+      </c>
+      <c r="D54" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D55" s="5" t="b">
         <v>0</v>
@@ -1479,27 +1458,27 @@
     </row>
     <row r="56" spans="1:5" ht="15.75" customHeight="1">
       <c r="A56" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D56" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" customHeight="1">
       <c r="A57" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D57" s="5" t="b">
         <v>1</v>
@@ -1507,83 +1486,83 @@
     </row>
     <row r="58" spans="1:5" ht="15.75" customHeight="1">
       <c r="A58" s="3" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D58" t="b">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="D58" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" customHeight="1">
       <c r="A59" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" customHeight="1">
       <c r="A60" s="3" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D60" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15.75" customHeight="1">
       <c r="A61" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="15.75" customHeight="1">
       <c r="A62" s="3" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15.75" customHeight="1">
       <c r="A63" s="3" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
@@ -1591,13 +1570,13 @@
     </row>
     <row r="64" spans="1:5" ht="15.75" customHeight="1">
       <c r="A64" s="3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
@@ -1605,13 +1584,13 @@
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1">
       <c r="A65" s="3" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
@@ -1619,13 +1598,13 @@
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1">
       <c r="A66" s="3" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -1633,13 +1612,13 @@
     </row>
     <row r="67" spans="1:4" ht="15.75" customHeight="1">
       <c r="A67" s="3" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D67" t="b">
         <v>0</v>
@@ -1647,13 +1626,13 @@
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1">
       <c r="A68" s="3" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D68" t="b">
         <v>0</v>
@@ -1661,13 +1640,13 @@
     </row>
     <row r="69" spans="1:4" ht="15.75" customHeight="1">
       <c r="A69" s="3" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D69" t="b">
         <v>0</v>
@@ -1675,49 +1654,77 @@
     </row>
     <row r="70" spans="1:4" ht="15.75" customHeight="1">
       <c r="A70" s="3" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D70" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" customHeight="1">
       <c r="A71" s="3" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1">
       <c r="A72" s="3" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D72" t="b">
         <v>0</v>
       </c>
     </row>
+    <row r="73" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A73" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A74" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E72">
-    <sortCondition ref="C2:C72"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E73">
+    <sortCondition ref="C2:C73"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
v0.4 changed some categorizations
</commit_message>
<xml_diff>
--- a/CAD Technology Radar.xlsx
+++ b/CAD Technology Radar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atitarenko/Documents/Code/TechRadar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096C5888-02AB-4A48-A3A8-AC692CEFE98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BE988A-A424-CC4C-98BD-EBCD773AC9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="93">
   <si>
     <t>name</t>
   </si>
@@ -310,6 +310,12 @@
   </si>
   <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>requirements not fulfilled for our team, otherwise a clear adopt</t>
+  </si>
+  <si>
+    <t>Carthage</t>
   </si>
 </sst>
 </file>
@@ -627,11 +633,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1310,7 +1316,7 @@
         <v>22</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>13</v>
@@ -1326,7 +1332,7 @@
         <v>Maestro</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>13</v>
@@ -1344,7 +1350,7 @@
         <v>OpenRewrite</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>13</v>
@@ -1523,13 +1529,16 @@
         <v>46</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D60" t="s">
         <v>90</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15.75" customHeight="1">
@@ -1725,6 +1734,20 @@
         <v>6</v>
       </c>
       <c r="D74" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A75" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D75" s="5" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v0.5 added more DIs and changed some categorizations
</commit_message>
<xml_diff>
--- a/CAD Technology Radar.xlsx
+++ b/CAD Technology Radar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atitarenko/Documents/Code/TechRadar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BE988A-A424-CC4C-98BD-EBCD773AC9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F863ACED-D669-4642-B76D-C96B4BDBCF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="95">
   <si>
     <t>name</t>
   </si>
@@ -316,6 +316,12 @@
   </si>
   <si>
     <t>Carthage</t>
+  </si>
+  <si>
+    <t>Dagger</t>
+  </si>
+  <si>
+    <t>Koin</t>
   </si>
 </sst>
 </file>
@@ -633,11 +639,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E73" sqref="E73"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -669,7 +675,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>18</v>
@@ -827,7 +833,7 @@
         <v>83</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>18</v>
@@ -855,7 +861,7 @@
         <v>45</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>18</v>
@@ -1748,6 +1754,34 @@
         <v>13</v>
       </c>
       <c r="D75" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A76" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A77" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D77" s="4" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated tech radar + added short description to every entry
</commit_message>
<xml_diff>
--- a/CAD Technology Radar.xlsx
+++ b/CAD Technology Radar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atitarenko/Documents/Code/TechRadar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F863ACED-D669-4642-B76D-C96B4BDBCF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4A6285-E3E0-424C-BE97-1AC1C382E843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="159">
   <si>
     <t>name</t>
   </si>
@@ -56,19 +56,12 @@
     <t>Techniques</t>
   </si>
   <si>
-    <t>&lt;p&gt;As application development becomes increasingly dynamic and complex, it's a challenge to deliver accessible and usable products with consistent style. This is particularly true in larger organizations with multiple teams working on different products. &lt;strong&gt;&lt;a href="https://www.thoughtworks.com/insights/decoder/d/design-systems"&gt;Design systems&lt;/a&gt;&lt;/strong&gt; define a collection of design patterns, component libraries and good design and engineering practices that ensure consistent digital products. Evolved from the corporate style guides of the past, design systems offer shared libraries and documents that are easy to find and use. Generally, guidance is written down as code and kept under version control so that the guide is less ambiguous and easier to maintain than simple documents. Design systems have become a standard approach when working across teams and disciplines in product development because they allow teams to focus. They can address strategic challenges around the product itself without reinventing the wheel every time a TRUE visual component is needed.&lt;/p&gt;
-&lt;p&gt;Our experiences show that teams seldom apply a product-centric mindset when building design systems. The primary consumers of the shared libraries and documents are the product development teams. When applying a product mindset, system owners should establish empathy with internal consumers (the development teams) and collaborate with them. We've found that the reason many component libraries are maligned is because the owning team wasn't able to give consumers what they needed fast enough and wasn't set up to take outside contributions. A product-centric mindset also requires organizations to think about if and how contributions should be made to the design system and how these contributions should be governed — on this topic, we recommend applying the &lt;a href="/radar/techniques/design-system-decision-records"&gt;design system decision records&lt;/a&gt; technique. For us, running a good design system or component library requires social work as much as technical work.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>Trial</t>
   </si>
   <si>
     <t>Assess</t>
   </si>
   <si>
-    <t>&lt;p&gt;As development of large language models continues, interest in building autonomous AI agents is strong. &lt;a href="https://github.com/Significant-Gravitas/Auto-GPT"&gt;AutoGPT&lt;/a&gt;, &lt;a href="https://github.com/AntonOsika/gpt-engineer"&gt;GPT-Engineer&lt;/a&gt; and &lt;a href="https://github.com/yoheinakajima/babyagi"&gt;BabyAGI&lt;/a&gt; are all examples of &lt;strong&gt;LLM-powered autonomous agents&lt;/strong&gt; that drive an underlying LLM to understand the goal they have been given and to work toward it. The agent remembers how far it has progressed, uses the LLM in order to reason about what to do next, takes actions and understands when the goal has been met. This is often known as chain-of-thought reasoning — and it can actually work. One of our teams implemented a client service chatbot as an autonomous agent. If the bot cannot achieve the customer's goal, it recognizes its own limitation and redirects the customer to a human instead. This approach is definitely early in its development cycle: autonomous agents often suffer from a high failure rate and incur costly AI service fees, and at least one AI startup has &lt;a href="https://twitter.com/zachtratar/status/1694024240880861571"&gt;pivoted away&lt;/a&gt; from an agent-based approach.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>Hold</t>
   </si>
   <si>
@@ -78,26 +71,9 @@
     <t>Tools</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;strong&gt;&lt;a href="https://github.com/features/copilot"&gt;GitHub Copilot&lt;/a&gt;&lt;/strong&gt; is used by many of our teams to help them write code faster. Overall, most of our developers find it very useful and would be cross if we took it away from them. We've been collating and sharing many of our experiences with Copilot through &lt;a href="https://martinfowler.com/articles/exploring-gen-ai.html"&gt;a series on Generative AI&lt;/a&gt; and &lt;a href="https://www.thoughtworks.com/insights/blog/generative-ai/getting-started-with-github-copilot"&gt;a guide on getting started with Copilot&lt;/a&gt;. Note that GitHub Copilot can be used with any codebase, not just codebases hosted on GitHub.&lt;/p&gt;
-&lt;p&gt;We're also excited that Copilot's chat feature from the &lt;a href="https://github.com/features/preview/copilot-x"&gt;Copilot X roadmap&lt;/a&gt; has become more widely available since we last featured it in the Radar. It is a powerful addition to Copilot's in-line assistance feature. The availability of a chat interface inside the IDE improves the discoverability of commonly searched information, and integration with the open editor context makes it easy to explore errors or ask the chat to assist with tasks related to the code in focus.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;&lt;a href="https://openai.com/blog/chatgpt"&gt;ChatGPT&lt;/a&gt;&lt;/strong&gt; continues to attract attention. Imaginative use cases and innovative approaches to prompting mean it's gaining expanding utility over time. GPT4, the large language model (LLM) that powers ChatGPT, now also has the ability to integrate with external tools such as a knowledge management repository, sandboxed coding environment or web search. The recent introduction of &lt;a href="https://openai.com/blog/introducing-chatgpt-enterprise"&gt;ChatGPT Enterprise&lt;/a&gt; may help ease intellectual property concerns, while providing "enterprise" features such as usage tracking and better user management through SSO.&lt;/p&gt;
-&lt;p&gt;Although ChatGPT's ability to "write" code has been much vaunted, we think organizations should be looking at using it across the full software lifecycle to improve efficiency and reduce errors. For example, ChatGPT can provide additional perspectives or suggestions for tasks as diverse as requirements analysis, architectural design or the reverse engineering of legacy systems. We still think ChatGPT is best used as an input to a process — such as helping with a first draft of a story or the boilerplate for a coding task — rather than a tool that produces "fully baked" results. That said, its capabilities are improving each week, and some programming tasks may now be fully possible by careful prompting, which is an &lt;a href="/radar/techniques/prompt-engineering"&gt;art in itself&lt;/a&gt;.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;&lt;a href="https://maestro.mobile.dev/"&gt;Maestro&lt;/a&gt;&lt;/strong&gt; is a TRUE cross-platform mobile UI test automation tool with built-in tolerance for flakiness and variance in application load times because of network or external factors. With a declarative YAML syntax, it makes it easy to write and maintain automated tests for mobile apps. It supports iOS and Android native apps, &lt;a href="/radar/languages-and-frameworks/react-native"&gt;React Native&lt;/a&gt; and &lt;a href="/radar/languages-and-frameworks/flutter"&gt;Flutter&lt;/a&gt; apps, as well as a variety of features for automating complex mobile UI interactions, such as tapping, scrolling and swiping. Maestro is distributed as a single binary for ease of use, runs in interpreted mode and makes it easy to author TRUE tests thanks to features like continuous mode. Maestro still lacks specific features like support for iOS devices, but the tool is rapidly evolving.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;We've seen several use cases for code intelligence tools: moving to a TRUE API version of a widely used library, understanding the impact of a just discovered vulnerability in such a library across an enterprise or applying updates to many services that were created from the same template. &lt;a href="/radar/tools/sourcegraph"&gt;Sourcegraph&lt;/a&gt; is still a popular tool in this space, and &lt;strong&gt;&lt;a href="https://github.com/openrewrite/rewrite"&gt;OpenRewrite&lt;/a&gt;&lt;/strong&gt; is another tool we want to highlight. While our teams have mostly used it in Java for narrow problems, like updating services created through a starter kit, it continues to broaden its coverage of languages and use cases. We like that it comes bundled with a catalog of recipes, which describe the changes to be made, for example for migrating commonly used frameworks across versions. The refactoring engine, bundled recipes and build tool plugins are open-source software, which makes it easier for teams to reach for OpenRewrite just when they need it. It remains to be seen how the maturing space of code intelligence tools, which are all based on parsing the source code into an abstract syntax tree (AST), will be impacted by the rapid developments in the space of LLMs.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>languages-and-frameworks</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;a href="https://github.com/Kotlin/kotlinx-kover"&gt;&lt;strong&gt;Kotlin Kover&lt;/strong&gt;&lt;/a&gt; is a code coverage tool set designed specifically for &lt;a href="/radar/languages-and-frameworks/kotlin"&gt;Kotlin&lt;/a&gt;, supporting Kotlin JVM, &lt;a href="/radar/languages-and-frameworks/kotlin-multiplatform-mobile"&gt;Multiplatform&lt;/a&gt; and Android projects. The significance of code coverage lies in its ability to spotlight untested segments, which reinforces software reliability. As Kover evolves, it stands out because of its ability to produce comprehensive HTML and XML reports, coupled with unmatched precision tailored to Kotlin. For teams deeply rooted in Kotlin, we advise you to assess Kover to leverage its potential in enhancing code quality.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>Unit testing</t>
   </si>
   <si>
@@ -197,9 +173,6 @@
     <t>Espresso</t>
   </si>
   <si>
-    <t>PowerMock</t>
-  </si>
-  <si>
     <t>OkHttp</t>
   </si>
   <si>
@@ -236,9 +209,6 @@
     <t>UI Component Display</t>
   </si>
   <si>
-    <t>Storybook for Apps</t>
-  </si>
-  <si>
     <t>AssertJ</t>
   </si>
   <si>
@@ -251,9 +221,6 @@
     <t>Crowdtesting</t>
   </si>
   <si>
-    <t>Testbirds</t>
-  </si>
-  <si>
     <t>Roadmap Planning</t>
   </si>
   <si>
@@ -287,9 +254,6 @@
     <t>Jetpack Compose</t>
   </si>
   <si>
-    <t>Jetpack Hilt</t>
-  </si>
-  <si>
     <t>Kotlin Coroutine</t>
   </si>
   <si>
@@ -299,36 +263,260 @@
     <t>TCA</t>
   </si>
   <si>
-    <t>Thread Modelling, OWASP Top 10, Security Champion, …</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;In a fast-paced product development environment where users' needs constantly evolve, design is an area that is ever-changing. This means input on design decisions will continue to be required. Borrowing from the idea of documenting architecture decisions via ADRs, we started adopting a similar format — &lt;strong&gt;design system decision records&lt;/strong&gt; — in order to document design system decisions with the corresponding rationale, research insights and experiment results. Communicating design system decisions effectively seems to be an emerging need of product development teams; doing it in this light manner is also recommended by &lt;a href="https://zeroheight.com/blog/capturing-your-design-system-decisions/"&gt;zeroheight&lt;/a&gt;. This technique helped us reduce onboarding times, move conversations forward and align work streams that share the same design system.&lt;/p&gt; 
-https://cognitect.com/blog/2011/11/15/documenting-architecture-decisions</t>
-  </si>
-  <si>
     <t>FALSE</t>
   </si>
   <si>
     <t>TRUE</t>
   </si>
   <si>
-    <t>requirements not fulfilled for our team, otherwise a clear adopt</t>
-  </si>
-  <si>
     <t>Carthage</t>
   </si>
   <si>
-    <t>Dagger</t>
-  </si>
-  <si>
     <t>Koin</t>
+  </si>
+  <si>
+    <t>Hilt</t>
+  </si>
+  <si>
+    <t>A mocking library for Kotlin to create and manage test doubles.</t>
+  </si>
+  <si>
+    <t>A modern, statically-typed programming language for JVM and Android development.</t>
+  </si>
+  <si>
+    <t>A powerful programming language for iOS, macOS, watchOS, and tvOS app development.</t>
+  </si>
+  <si>
+    <t>A declarative framework for building user interfaces across all Apple platforms.</t>
+  </si>
+  <si>
+    <t>A modern UI toolkit for building native Android interfaces using Kotlin.</t>
+  </si>
+  <si>
+    <t>React Native</t>
+  </si>
+  <si>
+    <t>A versatile, object-oriented programming language used for Android development.</t>
+  </si>
+  <si>
+    <t>A programming language primarily used for iOS and macOS apps before Swift.</t>
+  </si>
+  <si>
+    <t>An open-source UI framework for building cross-platform apps using Dart.</t>
+  </si>
+  <si>
+    <t>A service for sending push notifications to iOS, Android, and web applications.</t>
+  </si>
+  <si>
+    <t>A popular Java mocking framework for unit testing.</t>
+  </si>
+  <si>
+    <t>A framework for building user interfaces in iOS and macOS apps.</t>
+  </si>
+  <si>
+    <t>A component for managing app navigation in Android using a single activity.</t>
+  </si>
+  <si>
+    <t>A way to write Gradle build scripts using Kotlin instead of Groovy.</t>
+  </si>
+  <si>
+    <t>A tool for managing and distributing Swift code libraries.</t>
+  </si>
+  <si>
+    <t>A flexible testing framework for Kotlin that supports behavior-driven development.</t>
+  </si>
+  <si>
+    <t>A reactive programming framework for handling asynchronous events in Swift.</t>
+  </si>
+  <si>
+    <t>A set of libraries for composing asynchronous and event-based programs using observable sequences.</t>
+  </si>
+  <si>
+    <t>A Kotlin feature for simplifying asynchronous programming using lightweight threads.</t>
+  </si>
+  <si>
+    <t>A functional programming library for Kotlin, offering tools and patterns for handling data and effects.</t>
+  </si>
+  <si>
+    <t>Model-View-ViewModel; an architectural pattern that separates UI logic from business logic.</t>
+  </si>
+  <si>
+    <t>Model-View-Intent; a pattern that ensures a unidirectional data flow for predictable state management.</t>
+  </si>
+  <si>
+    <t>The Composable Architecture; a Swift architecture pattern focusing on composability and testability.</t>
+  </si>
+  <si>
+    <t>Model-View-Controller; a traditional pattern that divides an application into three interconnected components.</t>
+  </si>
+  <si>
+    <t>Model-View-Presenter; a pattern where the Presenter handles user input and updates the View.</t>
+  </si>
+  <si>
+    <t>A predictable state container for JavaScript apps, based on a unidirectional data flow.</t>
+  </si>
+  <si>
+    <t>A design pattern that promotes separation of concerns and independence from frameworks.</t>
+  </si>
+  <si>
+    <t>View-Interactor-Presenter-Entity-Router; a modular architecture pattern for apps.</t>
+  </si>
+  <si>
+    <t>A collection of reusable components and guidelines to create consistent design across applications.</t>
+  </si>
+  <si>
+    <t>A method for testing individual units of code to ensure they work as expected.</t>
+  </si>
+  <si>
+    <t>Secure Software Development Life Cycle; a process integrating security practices into every stage of software development.</t>
+  </si>
+  <si>
+    <t>Security Champion</t>
+  </si>
+  <si>
+    <t>Documentation of decisions made when developing or evolving a design system.</t>
+  </si>
+  <si>
+    <t>AI-driven agents using Large Language Models to perform tasks autonomously.</t>
+  </si>
+  <si>
+    <t>A strategy for rendering user interfaces on the server to enhance performance and security.</t>
+  </si>
+  <si>
+    <t>A software design that breaks down applications into smaller, interchangeable modules.</t>
+  </si>
+  <si>
+    <t>A team comprising members with different expertise (backend, web, app) working collaboratively.</t>
+  </si>
+  <si>
+    <t>A technique to enable or disable features in software without deploying new code.</t>
+  </si>
+  <si>
+    <t>Tools or rules that enforce consistent coding styles automatically.</t>
+  </si>
+  <si>
+    <t>A visual representation or library showcasing reusable UI components.</t>
+  </si>
+  <si>
+    <t>A logging practice that uses a consistent format to make logs easier to search and analyze.</t>
+  </si>
+  <si>
+    <t>A testing approach that leverages a large group of real users to test software in diverse environments.</t>
+  </si>
+  <si>
+    <t>The process of defining a strategic plan outlining future features, goals, and timelines for a product.</t>
+  </si>
+  <si>
+    <t>Managing the entire lifecycle of a product from planning and development to deployment and maintenance.</t>
+  </si>
+  <si>
+    <t>A Kotlin tool for measuring code coverage to help identify untested parts of an application.</t>
+  </si>
+  <si>
+    <t>A tool for continuous inspection of code quality to detect bugs, vulnerabilities, and code smells.</t>
+  </si>
+  <si>
+    <t>An open-source tool for end-to-end testing of mobile apps, offering powerful scripting capabilities.</t>
+  </si>
+  <si>
+    <t>An automated code refactoring tool for modernizing and improving Java applications.</t>
+  </si>
+  <si>
+    <t>An AI-powered code assistant that helps developers by suggesting code snippets and solutions.</t>
+  </si>
+  <si>
+    <t>An AI language model developed by OpenAI that can understand and generate human-like text.</t>
+  </si>
+  <si>
+    <t>A performance monitoring tool that provides real-time insights into application performance and user experience.</t>
+  </si>
+  <si>
+    <t>A mobile app security solution that protects apps from threats like reverse engineering and tampering.</t>
+  </si>
+  <si>
+    <t>A framework for creating customizable charts in iOS and macOS apps using Swift.</t>
+  </si>
+  <si>
+    <t>A library for rendering Adobe After Effects animations in real-time on various platforms.</t>
+  </si>
+  <si>
+    <t>An open-source tool for automating dependency updates in projects.</t>
+  </si>
+  <si>
+    <t>User interfaces enhanced by generative AI for personalized and dynamic user experiences.</t>
+  </si>
+  <si>
+    <t>An AI-powered tool that helps developers write, review, and maintain code with fewer bugs.</t>
+  </si>
+  <si>
+    <t>A static code analysis tool for Kotlin to detect code smells, style issues, and potential bugs.</t>
+  </si>
+  <si>
+    <t>An automation tool to streamline building, testing, and releasing mobile apps.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continuous Integration and Continuous Deployment pipelines hosted in the cloud to automate software delivery. </t>
+  </si>
+  <si>
+    <t>A memory leak detection library for Android apps.</t>
+  </si>
+  <si>
+    <t>A testing framework for writing concise, reliable Android UI tests.</t>
+  </si>
+  <si>
+    <t>A popular HTTP client library for Android and Java applications.</t>
+  </si>
+  <si>
+    <t>A charting library for Android to create beautiful and customizable data visualizations.</t>
+  </si>
+  <si>
+    <t>A type-safe HTTP client for Android and Java for managing REST API calls.</t>
+  </si>
+  <si>
+    <t>An image loading and caching library for Android that simplifies displaying images.</t>
+  </si>
+  <si>
+    <t>An Android library that provides an abstraction layer over SQLite to manage databases.</t>
+  </si>
+  <si>
+    <t>A modern JSON library for Android and Java for converting Java objects to JSON and vice versa.</t>
+  </si>
+  <si>
+    <t>A fluent assertions library for Java to write readable and expressive tests.</t>
+  </si>
+  <si>
+    <t>A build automation tool for Java, Android, and other JVM-based applications.</t>
+  </si>
+  <si>
+    <t>A popular Java library for processing JSON data, offering fast serialization and deserialization.</t>
+  </si>
+  <si>
+    <t>A method of comparing two or more versions of a feature or product to determine which performs better.</t>
+  </si>
+  <si>
+    <t>A decentralized dependency manager for iOS projects, using Swift and Objective-C.</t>
+  </si>
+  <si>
+    <t>A dependency injection library for Android, built on top of Dagger, to simplify dependency management.</t>
+  </si>
+  <si>
+    <t>A lightweight dependency injection framework for Kotlin, designed to be simple and pragmatic.</t>
+  </si>
+  <si>
+    <t>A framework for building cross-platform mobile apps using JavaScript and React.</t>
+  </si>
+  <si>
+    <t>A role within a team that advocates for security best practices and helps identify potential vulnerabilities.</t>
+  </si>
+  <si>
+    <t>Access Integration &amp; Delivery Automation pipelines hosted at 1&amp;1 to automate software delivery. Hold because of many drawbacks for app development.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -370,13 +558,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -404,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -414,13 +595,7 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -642,15 +817,15 @@
   <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="51.5" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" customWidth="1"/>
-    <col min="5" max="5" width="130.33203125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="130.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17">
@@ -672,405 +847,487 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="13">
       <c r="A13" s="3" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>89</v>
+        <v>12</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="13">
       <c r="A14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="13">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>89</v>
+        <v>77</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>76</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>77</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" t="s">
-        <v>90</v>
+        <v>5</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>89</v>
+        <v>77</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>90</v>
+        <v>10</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>89</v>
+        <v>10</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A29" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A30" s="3" t="str">
+      <c r="A29" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/techniques/design-systems","Design systems")</f>
         <v>Design systems</v>
       </c>
+      <c r="B29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A30" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="B30" s="4" t="s">
         <v>5</v>
       </c>
@@ -1078,15 +1335,15 @@
         <v>6</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>7</v>
+        <v>76</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>5</v>
@@ -1095,31 +1352,34 @@
         <v>6</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E31" s="9"/>
+        <v>76</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A32" s="3" t="s">
-        <v>23</v>
+      <c r="A32" s="3" t="str">
+        <f>HYPERLINK("https://www.thoughtworks.com/radar/techniques/design-system-decision-records","Design system decision records")</f>
+        <v>Design system decision records</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>87</v>
+        <v>77</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1">
       <c r="A33" s="3" t="str">
-        <f>HYPERLINK("https://www.thoughtworks.com/radar/techniques/design-system-decision-records","Design system decision records")</f>
-        <v>Design system decision records</v>
+        <f>HYPERLINK("https://www.thoughtworks.com/radar/techniques/llm-powered-autonomous-agents","LLM-powered autonomous agents")</f>
+        <v>LLM-powered autonomous agents</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>8</v>
@@ -1128,90 +1388,100 @@
         <v>6</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>88</v>
+        <v>77</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A34" s="3" t="str">
-        <f>HYPERLINK("https://www.thoughtworks.com/radar/techniques/llm-powered-autonomous-agents","LLM-powered autonomous agents")</f>
-        <v>LLM-powered autonomous agents</v>
+      <c r="A34" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>10</v>
+        <v>77</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E35" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" t="s">
-        <v>90</v>
+        <v>6</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>90</v>
+      <c r="D37" t="s">
+        <v>76</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A38" s="3" t="s">
-        <v>63</v>
+      <c r="A38" t="s">
+        <v>56</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A39" t="s">
-        <v>64</v>
+      <c r="A39" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>8</v>
@@ -1220,43 +1490,49 @@
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>89</v>
+        <v>77</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1">
       <c r="A40" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>90</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>66</v>
+        <v>76</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1">
       <c r="A42" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>5</v>
@@ -1265,15 +1541,15 @@
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>89</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>71</v>
+        <v>76</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1">
       <c r="A43" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>5</v>
@@ -1282,512 +1558,598 @@
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A44" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A45" s="3" t="str">
+      <c r="A44" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/languages-and-frameworks/kotlin-kover","Kotlin Kover")</f>
         <v>Kotlin Kover</v>
       </c>
+      <c r="B44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A45" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="B45" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>19</v>
+        <v>76</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A46" s="3" t="s">
-        <v>22</v>
+      <c r="A46" s="3" t="str">
+        <f>HYPERLINK("https://www.thoughtworks.com/radar/tools/maestro","Maestro")</f>
+        <v>Maestro</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E46" s="7"/>
+        <v>77</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1">
       <c r="A47" s="3" t="str">
-        <f>HYPERLINK("https://www.thoughtworks.com/radar/tools/maestro","Maestro")</f>
-        <v>Maestro</v>
+        <f>HYPERLINK("https://www.thoughtworks.com/radar/tools/openrewrite","OpenRewrite")</f>
+        <v>OpenRewrite</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>16</v>
+        <v>77</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" customHeight="1">
       <c r="A48" s="3" t="str">
-        <f>HYPERLINK("https://www.thoughtworks.com/radar/tools/openrewrite","OpenRewrite")</f>
-        <v>OpenRewrite</v>
+        <f>HYPERLINK("https://www.thoughtworks.com/radar/tools/github-copilot","GitHub Copilot")</f>
+        <v>GitHub Copilot</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>17</v>
+        <v>76</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75" customHeight="1">
       <c r="A49" s="3" t="str">
-        <f>HYPERLINK("https://www.thoughtworks.com/radar/tools/github-copilot","GitHub Copilot")</f>
-        <v>GitHub Copilot</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A50" s="3" t="str">
         <f>HYPERLINK("https://www.thoughtworks.com/radar/tools/chatgpt","ChatGPT")</f>
         <v>ChatGPT</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>8</v>
+      <c r="B49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A50" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>15</v>
+        <v>76</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A53" s="3" t="s">
-        <v>38</v>
+      <c r="A53" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A54" s="5" t="s">
-        <v>62</v>
+      <c r="A54" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>89</v>
+        <v>11</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15.75" customHeight="1">
       <c r="A56" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>89</v>
+        <v>77</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" customHeight="1">
       <c r="A57" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>90</v>
+        <v>77</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15.75" customHeight="1">
       <c r="A58" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>90</v>
+        <v>11</v>
+      </c>
+      <c r="D58" t="s">
+        <v>76</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" customHeight="1">
       <c r="A59" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D59" t="s">
-        <v>89</v>
+        <v>77</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" customHeight="1">
       <c r="A60" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D60" t="s">
-        <v>90</v>
-      </c>
-      <c r="E60" s="10" t="s">
-        <v>91</v>
+        <v>76</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15.75" customHeight="1">
       <c r="A61" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D61" t="s">
-        <v>89</v>
+        <v>77</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="15.75" customHeight="1">
       <c r="A62" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D62" t="s">
-        <v>90</v>
+        <v>76</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15.75" customHeight="1">
       <c r="A63" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D63" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="15.75" customHeight="1">
       <c r="A64" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D64" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="15.75" customHeight="1">
+        <v>76</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15.75" customHeight="1">
       <c r="A65" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D65" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="15.75" customHeight="1">
+        <v>76</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" customHeight="1">
       <c r="A66" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D66" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="15.75" customHeight="1">
+        <v>76</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15.75" customHeight="1">
       <c r="A67" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D67" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="15.75" customHeight="1">
+        <v>76</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15.75" customHeight="1">
       <c r="A68" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D68" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="15.75" customHeight="1">
+        <v>76</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" customHeight="1">
       <c r="A69" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B69" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" t="s">
+        <v>77</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A70" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" t="s">
+        <v>76</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A71" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D71" t="s">
+        <v>76</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A72" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" t="s">
+        <v>76</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A73" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A74" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A75" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D69" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A70" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D70" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A71" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D71" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A72" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D72" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A73" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D73" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A74" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C74" s="5" t="s">
+      <c r="C75" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A76" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A77" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D74" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A75" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A76" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A77" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>89</v>
+      <c r="D77" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E73">
-    <sortCondition ref="C2:C73"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E71">
+    <sortCondition ref="C2:C71"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>